<commit_message>
Clean of functions notebook
</commit_message>
<xml_diff>
--- a/predictions/predictions.xlsx
+++ b/predictions/predictions.xlsx
@@ -654,7 +654,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1406,7 +1406,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2094,7 +2094,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2270,7 +2270,7 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2998,7 +2998,7 @@
         <v>326</v>
       </c>
       <c r="B328">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -4470,7 +4470,7 @@
         <v>510</v>
       </c>
       <c r="B512">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="513" spans="1:2">
@@ -5062,7 +5062,7 @@
         <v>584</v>
       </c>
       <c r="B586">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="587" spans="1:2">
@@ -6382,7 +6382,7 @@
         <v>749</v>
       </c>
       <c r="B751">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="752" spans="1:2">
@@ -6470,7 +6470,7 @@
         <v>760</v>
       </c>
       <c r="B762">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="763" spans="1:2">
@@ -6478,7 +6478,7 @@
         <v>761</v>
       </c>
       <c r="B763">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="764" spans="1:2">
@@ -6718,7 +6718,7 @@
         <v>791</v>
       </c>
       <c r="B793">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:2">
@@ -6870,7 +6870,7 @@
         <v>810</v>
       </c>
       <c r="B812">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="813" spans="1:2">
@@ -7134,7 +7134,7 @@
         <v>843</v>
       </c>
       <c r="B845">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="846" spans="1:2">
@@ -7334,7 +7334,7 @@
         <v>868</v>
       </c>
       <c r="B870">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="871" spans="1:2">
@@ -8534,7 +8534,7 @@
         <v>1018</v>
       </c>
       <c r="B1020">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1021" spans="1:2">
@@ -8726,7 +8726,7 @@
         <v>1042</v>
       </c>
       <c r="B1044">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1045" spans="1:2">
@@ -9534,7 +9534,7 @@
         <v>1143</v>
       </c>
       <c r="B1145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1146" spans="1:2">
@@ -10798,7 +10798,7 @@
         <v>1301</v>
       </c>
       <c r="B1303">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1304" spans="1:2">
@@ -10918,7 +10918,7 @@
         <v>1316</v>
       </c>
       <c r="B1318">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1319" spans="1:2">
@@ -11198,7 +11198,7 @@
         <v>1351</v>
       </c>
       <c r="B1353">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1354" spans="1:2">
@@ -11246,7 +11246,7 @@
         <v>1357</v>
       </c>
       <c r="B1359">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1360" spans="1:2">
@@ -11462,7 +11462,7 @@
         <v>1384</v>
       </c>
       <c r="B1386">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1387" spans="1:2">
@@ -11782,7 +11782,7 @@
         <v>1424</v>
       </c>
       <c r="B1426">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1427" spans="1:2">
@@ -12382,7 +12382,7 @@
         <v>1499</v>
       </c>
       <c r="B1501">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1502" spans="1:2">
@@ -12550,7 +12550,7 @@
         <v>1520</v>
       </c>
       <c r="B1522">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1523" spans="1:2">
@@ -12910,7 +12910,7 @@
         <v>1565</v>
       </c>
       <c r="B1567">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1568" spans="1:2">
@@ -13014,7 +13014,7 @@
         <v>1578</v>
       </c>
       <c r="B1580">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1581" spans="1:2">
@@ -14150,7 +14150,7 @@
         <v>1720</v>
       </c>
       <c r="B1722">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1723" spans="1:2">
@@ -14294,7 +14294,7 @@
         <v>1738</v>
       </c>
       <c r="B1740">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1741" spans="1:2">
@@ -15062,7 +15062,7 @@
         <v>1834</v>
       </c>
       <c r="B1836">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1837" spans="1:2">
@@ -15078,7 +15078,7 @@
         <v>1836</v>
       </c>
       <c r="B1838">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1839" spans="1:2">
@@ -15942,7 +15942,7 @@
         <v>1944</v>
       </c>
       <c r="B1946">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1947" spans="1:2">
@@ -17134,7 +17134,7 @@
         <v>2093</v>
       </c>
       <c r="B2095">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2096" spans="1:2">
@@ -17470,7 +17470,7 @@
         <v>2135</v>
       </c>
       <c r="B2137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2138" spans="1:2">
@@ -18246,7 +18246,7 @@
         <v>2232</v>
       </c>
       <c r="B2234">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2235" spans="1:2">
@@ -19326,7 +19326,7 @@
         <v>2367</v>
       </c>
       <c r="B2369">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2370" spans="1:2">
@@ -19478,7 +19478,7 @@
         <v>2386</v>
       </c>
       <c r="B2388">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2389" spans="1:2">
@@ -19502,7 +19502,7 @@
         <v>2389</v>
       </c>
       <c r="B2391">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2392" spans="1:2">
@@ -19950,7 +19950,7 @@
         <v>2445</v>
       </c>
       <c r="B2447">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2448" spans="1:2">
@@ -20030,7 +20030,7 @@
         <v>2455</v>
       </c>
       <c r="B2457">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2458" spans="1:2">
@@ -20126,7 +20126,7 @@
         <v>2467</v>
       </c>
       <c r="B2469">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2470" spans="1:2">
@@ -20150,7 +20150,7 @@
         <v>2470</v>
       </c>
       <c r="B2472">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2473" spans="1:2">
@@ -20246,7 +20246,7 @@
         <v>2482</v>
       </c>
       <c r="B2484">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2485" spans="1:2">
@@ -20574,7 +20574,7 @@
         <v>2523</v>
       </c>
       <c r="B2525">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2526" spans="1:2">
@@ -20702,7 +20702,7 @@
         <v>2539</v>
       </c>
       <c r="B2541">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2542" spans="1:2">
@@ -20950,7 +20950,7 @@
         <v>2570</v>
       </c>
       <c r="B2572">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2573" spans="1:2">
@@ -21086,7 +21086,7 @@
         <v>2587</v>
       </c>
       <c r="B2589">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2590" spans="1:2">
@@ -21214,7 +21214,7 @@
         <v>2603</v>
       </c>
       <c r="B2605">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2606" spans="1:2">
@@ -21262,7 +21262,7 @@
         <v>2609</v>
       </c>
       <c r="B2611">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2612" spans="1:2">
@@ -21550,7 +21550,7 @@
         <v>2645</v>
       </c>
       <c r="B2647">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2648" spans="1:2">
@@ -22350,7 +22350,7 @@
         <v>2745</v>
       </c>
       <c r="B2747">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2748" spans="1:2">
@@ -23118,7 +23118,7 @@
         <v>2841</v>
       </c>
       <c r="B2843">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2844" spans="1:2">
@@ -23398,7 +23398,7 @@
         <v>2876</v>
       </c>
       <c r="B2878">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2879" spans="1:2">
@@ -23862,7 +23862,7 @@
         <v>2934</v>
       </c>
       <c r="B2936">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2937" spans="1:2">
@@ -24182,7 +24182,7 @@
         <v>2974</v>
       </c>
       <c r="B2976">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2977" spans="1:2">
@@ -24710,7 +24710,7 @@
         <v>3040</v>
       </c>
       <c r="B3042">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3043" spans="1:2">
@@ -25230,7 +25230,7 @@
         <v>3105</v>
       </c>
       <c r="B3107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3108" spans="1:2">
@@ -25990,7 +25990,7 @@
         <v>3200</v>
       </c>
       <c r="B3202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3203" spans="1:2">
@@ -26270,7 +26270,7 @@
         <v>3235</v>
       </c>
       <c r="B3237">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3238" spans="1:2">
@@ -27118,7 +27118,7 @@
         <v>3341</v>
       </c>
       <c r="B3343">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3344" spans="1:2">
@@ -27406,7 +27406,7 @@
         <v>3377</v>
       </c>
       <c r="B3379">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3380" spans="1:2">
@@ -27590,7 +27590,7 @@
         <v>3400</v>
       </c>
       <c r="B3402">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3403" spans="1:2">
@@ -27646,7 +27646,7 @@
         <v>3407</v>
       </c>
       <c r="B3409">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3410" spans="1:2">
@@ -27774,7 +27774,7 @@
         <v>3423</v>
       </c>
       <c r="B3425">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3426" spans="1:2">
@@ -28718,7 +28718,7 @@
         <v>3541</v>
       </c>
       <c r="B3543">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3544" spans="1:2">
@@ -28766,7 +28766,7 @@
         <v>3547</v>
       </c>
       <c r="B3549">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3550" spans="1:2">
@@ -30550,7 +30550,7 @@
         <v>3770</v>
       </c>
       <c r="B3772">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3773" spans="1:2">
@@ -30598,7 +30598,7 @@
         <v>3776</v>
       </c>
       <c r="B3778">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3779" spans="1:2">
@@ -30654,7 +30654,7 @@
         <v>3783</v>
       </c>
       <c r="B3785">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3786" spans="1:2">
@@ -31070,7 +31070,7 @@
         <v>3835</v>
       </c>
       <c r="B3837">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3838" spans="1:2">
@@ -31190,7 +31190,7 @@
         <v>3850</v>
       </c>
       <c r="B3852">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3853" spans="1:2">
@@ -31350,7 +31350,7 @@
         <v>3870</v>
       </c>
       <c r="B3872">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3873" spans="1:2">
@@ -31958,7 +31958,7 @@
         <v>3946</v>
       </c>
       <c r="B3948">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3949" spans="1:2">
@@ -31990,7 +31990,7 @@
         <v>3950</v>
       </c>
       <c r="B3952">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3953" spans="1:2">
@@ -32078,7 +32078,7 @@
         <v>3961</v>
       </c>
       <c r="B3963">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3964" spans="1:2">
@@ -32118,7 +32118,7 @@
         <v>3966</v>
       </c>
       <c r="B3968">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3969" spans="1:2">
@@ -32502,7 +32502,7 @@
         <v>4014</v>
       </c>
       <c r="B4016">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4017" spans="1:2">
@@ -32630,7 +32630,7 @@
         <v>4030</v>
       </c>
       <c r="B4032">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4033" spans="1:2">
@@ -33102,7 +33102,7 @@
         <v>4089</v>
       </c>
       <c r="B4091">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4092" spans="1:2">
@@ -33566,7 +33566,7 @@
         <v>4147</v>
       </c>
       <c r="B4149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4150" spans="1:2">
@@ -33606,7 +33606,7 @@
         <v>4152</v>
       </c>
       <c r="B4154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4155" spans="1:2">

</xml_diff>